<commit_message>
combined new data with old one
</commit_message>
<xml_diff>
--- a/data/Forensic Trafficking Interviews Question Type Examples 10_1_24.xlsx
+++ b/data/Forensic Trafficking Interviews Question Type Examples 10_1_24.xlsx
@@ -182,7 +182,7 @@
     <t>question code</t>
   </si>
   <si>
-    <t>label</t>
+    <t>Label</t>
   </si>
   <si>
     <t>NICHD</t>
@@ -9383,7 +9383,7 @@
   <dimension ref="A1:O1180"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5037037037037" defaultRowHeight="15" customHeight="1"/>

</xml_diff>